<commit_message>
Modified structure of code
</commit_message>
<xml_diff>
--- a/assets/CMS Template.xlsx
+++ b/assets/CMS Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C2D226-D86F-452E-A053-94D2A5F6C7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBB770C-6BA8-4F75-9A2E-46B9E131D3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="1540" windowWidth="8460" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -374,6 +374,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -387,9 +390,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -716,10 +716,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="24"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -769,11 +769,11 @@
       <c r="B7" s="12"/>
     </row>
     <row r="8" spans="1:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="A8" s="24" t="str">
+      <c r="A8" s="25" t="str">
         <f>$B$2 &amp; " Only"</f>
         <v>Professional (CMS) Only</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="26"/>
     </row>
     <row r="9" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A9" s="9" t="str">
@@ -869,7 +869,7 @@
       <c r="B19" s="12"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B20" s="27"/>
+      <c r="B20" s="22"/>
     </row>
     <row r="21" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
@@ -972,10 +972,10 @@
       <c r="J1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="26"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
@@ -1074,7 +1074,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Rename via pdf name instead of most recent
</commit_message>
<xml_diff>
--- a/assets/CMS Template.xlsx
+++ b/assets/CMS Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kai\Desktop\ClaimBot\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBB770C-6BA8-4F75-9A2E-46B9E131D3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF49415-4D2E-41B1-9824-2ECF5C0927A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Range</t>
+  </si>
+  <si>
+    <t>McGee, Test</t>
+  </si>
+  <si>
+    <t>5/1/24 - 5/18/24</t>
+  </si>
+  <si>
+    <t>Anna, Mary</t>
   </si>
 </sst>
 </file>
@@ -877,7 +886,7 @@
       </c>
       <c r="B21" s="16">
         <f>COUNTA(Claims!A:A)-1</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
@@ -886,7 +895,7 @@
       </c>
       <c r="B22" s="13">
         <f>SUMIF(Claims!D:D, "&gt;0")</f>
-        <v>0</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
@@ -1074,7 +1083,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:C6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1103,10 +1112,32 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="21"/>
+      <c r="A2" s="21">
+        <v>45430</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1235</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="21"/>
+      <c r="A3" s="21">
+        <v>45430</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5">
+        <v>380</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="21"/>

</xml_diff>